<commit_message>
deleted fields{project name, meter reading id} from the template, modified document accordingly
</commit_message>
<xml_diff>
--- a/Code/converter/PMfile/template.xlsx
+++ b/Code/converter/PMfile/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baozi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SEED\gitDir\SEEDproject\Code\converter\PMfile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,23 +24,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Street Address</t>
   </si>
   <si>
-    <t>Project Name</t>
-  </si>
-  <si>
     <t>Portfolio Manager Meter ID</t>
   </si>
   <si>
     <t>Meter Type</t>
   </si>
   <si>
-    <t>Meter Consumption ID</t>
-  </si>
-  <si>
     <t>Start Date</t>
   </si>
   <si>
@@ -60,9 +54,6 @@
   </si>
   <si>
     <t>Natural Gas</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
   <si>
     <t>5000 Forbes Ave</t>
@@ -72,6 +63,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="m/d/yy\ h:mm;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -109,13 +103,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,33 +390,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -440,46 +432,35 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4674008</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3">
+        <v>41944</v>
+      </c>
+      <c r="E2" s="3">
+        <v>41974</v>
+      </c>
+      <c r="F2">
+        <v>100000</v>
+      </c>
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2">
-        <v>4674008</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2">
-        <v>16873474</v>
-      </c>
-      <c r="F2" s="1">
-        <v>41944</v>
-      </c>
-      <c r="G2" s="1">
-        <v>41974</v>
-      </c>
       <c r="H2">
-        <v>100000</v>
-      </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2">
         <v>9000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>